<commit_message>
Semi-final version cubic spline
</commit_message>
<xml_diff>
--- a/Excel_CHECK.xlsx
+++ b/Excel_CHECK.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\Numerical_Methods\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Maestria\Nummerical Methods\Group Assignment\Numerical_Methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C2337A-1A38-4357-8ACA-FD5A6D20B86A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E408437E-8D24-4390-A462-A95C00518DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AA5CC8F3-D55D-4CE5-995D-840FC6E3257C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{AA5CC8F3-D55D-4CE5-995D-840FC6E3257C}"/>
   </bookViews>
   <sheets>
     <sheet name="Newton's Method" sheetId="1" r:id="rId1"/>
@@ -36,8 +36,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>Newton's Method</t>
   </si>
@@ -119,11 +141,38 @@
   <si>
     <t>r=</t>
   </si>
+  <si>
+    <t>M^-1=</t>
+  </si>
+  <si>
+    <t>c=</t>
+  </si>
+  <si>
+    <t>b=</t>
+  </si>
+  <si>
+    <t>d=</t>
+  </si>
+  <si>
+    <t>c0=</t>
+  </si>
+  <si>
+    <t>cn=</t>
+  </si>
+  <si>
+    <t>Expected</t>
+  </si>
+  <si>
+    <t>Real</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -208,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -219,6 +268,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -236,6 +288,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -634,8 +693,11 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Series2</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:noFill/>
@@ -648,11 +710,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -721,7 +783,1320 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-58B7-433A-9E91-5E8C457A562C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1284429311"/>
+        <c:axId val="1905474127"/>
+      </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Expected</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Cubic Spline'!$B$44:$B$144</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-5.88</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-5.76</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-5.64</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-5.52</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-5.3999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-5.2799999999999994</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-5.1599999999999993</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-5.0399999999999991</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-4.919999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-4.7999999999999989</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-4.6799999999999988</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-4.5599999999999987</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-4.4399999999999986</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-4.3199999999999985</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-4.1999999999999984</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-4.0799999999999983</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-3.9599999999999982</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-3.8399999999999981</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-3.719999999999998</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-3.5999999999999979</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-3.4799999999999978</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-3.3599999999999977</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-3.2399999999999975</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-3.1199999999999974</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-2.9999999999999973</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-2.8799999999999972</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-2.7599999999999971</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-2.639999999999997</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-2.5199999999999969</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-2.3999999999999968</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-2.2799999999999967</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-2.1599999999999966</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-2.0399999999999965</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-1.9199999999999964</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-1.7999999999999963</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-1.6799999999999962</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-1.5599999999999961</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-1.4399999999999959</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-1.3199999999999958</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-1.1999999999999957</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-1.0799999999999956</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-0.95999999999999563</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-0.83999999999999564</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-0.71999999999999564</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-0.59999999999999565</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-0.47999999999999565</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-0.35999999999999566</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-0.23999999999999566</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-0.11999999999999567</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4.3298697960381105E-15</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.12000000000000433</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.24000000000000432</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.36000000000000432</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.48000000000000431</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.60000000000000431</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.7200000000000043</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.8400000000000043</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.96000000000000429</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.0800000000000043</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1.2000000000000042</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.3200000000000043</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.4400000000000044</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.5600000000000045</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.6800000000000046</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1.8000000000000047</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1.9200000000000048</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2.0400000000000049</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2.160000000000005</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2.2800000000000051</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2.4000000000000052</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2.5200000000000053</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2.6400000000000055</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2.7600000000000056</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2.8800000000000057</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>3.0000000000000058</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>3.1200000000000059</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>3.240000000000006</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>3.3600000000000061</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>3.4800000000000062</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>3.6000000000000063</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>3.7200000000000064</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>3.8400000000000065</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>3.9600000000000066</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>4.0800000000000063</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>4.2000000000000064</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>4.3200000000000065</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>4.4400000000000066</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>4.5600000000000067</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>4.6800000000000068</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>4.8000000000000069</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>4.920000000000007</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>5.0400000000000071</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>5.1600000000000072</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>5.2800000000000074</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>5.4000000000000075</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>5.5200000000000076</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>5.6400000000000077</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>5.7600000000000078</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>5.8800000000000079</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>6.000000000000008</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Cubic Spline'!$C$44:$C$144</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>2.5289999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5208001179076924</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5117738663384617</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5010948758153844</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.4879367768615386</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.4714732000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.4508777757538462</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.4253241346461536</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.3939859071999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.3560367239384608</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.3106502153846145</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.2570000120615377</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.1942597444923067</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.121603043199999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.0382035387076911</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.94323486153846</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.8358706422153828</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.7153019655384596</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.5817671729230747</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.4371278535384588</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.2833852307692279</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.1225405279999969</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.95659496861538129</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.78754977599999643</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.61740617353845784</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.44816538461538091</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.28182863261538077</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.12039714092307313</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-3.4127867076926943E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-0.17974516800000384</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-0.31445353846154189</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-0.43625175507692637</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-0.54313859446154145</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-0.63311283323077228</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-0.70432455286154039</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-0.75668275384615524</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-0.79123122313846239</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-0.80903266080000036</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-0.81114976689230756</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-0.79864524147692229</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-0.77258178461538352</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-0.73402209636922922</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-0.68402887679999813</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-0.62366482596922834</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-0.55399264393845893</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-0.47607503076922791</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-0.39097468652307354</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-0.29975431126153523</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-0.20347660504615062</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-0.10320426793845783</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>3.7639558136959306E-15</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.10506934486154226</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.21092029735384996</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.3164652343384653</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.42061653267692678</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.52228656923077277</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.62038772086154181</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.71383236443077247</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.80153287680000296</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.88240163483077194</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.95535101538461786</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.0192933953230792</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.0731411515076941</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.1158066608000015</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.1462023000615393</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1.1632404461538466</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1.1658334759384612</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.15291329476923</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.1245835175384602</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1.0827639089230747</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1.0295304615384588</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.96695916799999704</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.8971260209230737</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.82210701292307342</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.74397813661538093</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.66481538461538081</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.58669474953845779</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.51169222399999637</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.44188380061538113</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.37934547199999702</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.3261532307692282</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.28438306953845971</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.2561109809230756</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.24341295753846093</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.24820812701538533</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.27059206153846316</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.30948384590769484</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.36378295680000344</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.43238887089231198</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.51420106486154349</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.60811901538462121</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.71304219913846822</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.82787009280000723</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.9515021730461618</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1.0828379165538544</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>1.220776800000009</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>1.364218300061548</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>1.5120618934153944</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>1.6632070567384716</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>1.8165532667077025</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>1.9710000000000107</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-A4F9-4782-9ACA-8EF0101C2FB5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Real</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Cubic Spline'!$D$44:$D$144</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-5.88</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-5.76</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-5.64</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-5.52</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-5.3999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-5.2799999999999994</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-5.1599999999999993</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-5.0399999999999991</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-4.919999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-4.7999999999999989</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-4.6799999999999988</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-4.5599999999999987</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-4.4399999999999986</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-4.3199999999999985</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-4.1999999999999984</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-4.0799999999999983</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-3.9599999999999982</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-3.8399999999999981</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-3.719999999999998</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-3.5999999999999979</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-3.4799999999999978</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-3.3599999999999977</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-3.2399999999999975</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-3.1199999999999974</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-2.9999999999999973</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-2.8799999999999972</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-2.7599999999999971</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-2.639999999999997</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-2.5199999999999969</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-2.3999999999999968</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-2.2799999999999967</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-2.1599999999999966</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-2.0399999999999965</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-1.9199999999999964</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-1.7999999999999963</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-1.6799999999999962</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-1.5599999999999961</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-1.4399999999999959</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-1.3199999999999958</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-1.1999999999999957</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-1.0799999999999956</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-0.95999999999999563</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-0.83999999999999564</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-0.71999999999999564</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-0.59999999999999565</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-0.47999999999999565</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-0.35999999999999566</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-0.23999999999999566</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-0.11999999999999567</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4.3298697960381105E-15</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.12000000000000433</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.24000000000000432</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.36000000000000432</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.48000000000000431</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.60000000000000431</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.7200000000000043</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.8400000000000043</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.96000000000000429</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.0800000000000043</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1.2000000000000042</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.3200000000000043</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.4400000000000044</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.5600000000000045</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.6800000000000046</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1.8000000000000047</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1.9200000000000048</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2.0400000000000049</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2.160000000000005</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2.2800000000000051</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2.4000000000000052</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2.5200000000000053</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2.6400000000000055</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2.7600000000000056</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2.8800000000000057</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>3.0000000000000058</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>3.1200000000000059</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>3.240000000000006</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>3.3600000000000061</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>3.4800000000000062</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>3.6000000000000063</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>3.7200000000000064</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>3.8400000000000065</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>3.9600000000000066</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>4.0800000000000063</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>4.2000000000000064</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>4.3200000000000065</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>4.4400000000000066</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>4.5600000000000067</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>4.6800000000000068</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>4.8000000000000069</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>4.920000000000007</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>5.0400000000000071</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>5.1600000000000072</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>5.2800000000000074</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>5.4000000000000075</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>5.5200000000000076</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>5.6400000000000077</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>5.7600000000000078</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>5.8800000000000079</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>6.000000000000008</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Cubic Spline'!$E$44:$E$144</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>2.5289999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5208001000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5117737999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5010948000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.4879367000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.4714732000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.4508779000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.4253241999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.3939859999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.3560367000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.3106502999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.2570000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.1942596000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.1216029999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.0382037</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.9432347000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.8358705</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.7153020000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.5817673000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.4371278000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.2833854</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.1225404999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.95659506000000005</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.78754972999999995</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.61740625000000005</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.44816529999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.28182869999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.12039704</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-3.41278203E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-0.17974527000000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-0.31445350999999999</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-0.43625185</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-0.54313856000000005</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-0.63311273000000001</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-0.70432448000000003</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-0.75668274999999996</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-0.79123122000000001</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-0.80903267999999995</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-0.81114978000000004</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-0.79864526000000002</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-0.77258181999999997</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-0.73402219999999996</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-0.68402898000000001</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-0.62366491999999996</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-0.55399281</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-0.47607519999999998</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-0.39097484999999998</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-0.29975447</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-0.20347677</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-0.10320443999999999</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-1.7618685900000001E-7</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.10506923</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.21092018000000001</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.31646510999999999</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.42061641999999999</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.52228646999999995</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.62038760999999998</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.71383226</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.80153280000000005</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.88240152999999999</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.95535093999999998</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.0192933</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.0731411</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.1158067</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.1462022999999999</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1.1632406</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1.1658336</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.1529133</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.1245836</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1.0827640000000001</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1.0295304999999999</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.96695936000000005</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.89712614000000002</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.82210720000000004</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.74397826</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.66481555000000003</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.58669484000000005</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.51169240000000005</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.44188386000000002</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.37934560000000001</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.32615327999999999</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.28438314999999997</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.25611106</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.24341297000000001</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.24820812</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.270592</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.30948371000000002</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.36378273</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.43238881000000001</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.51420093</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.60811877000000003</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.71304177999999996</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.82787001000000005</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.95150197000000003</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1.0828376</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>1.2207763</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>1.3642175999999999</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>1.5120617000000001</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>1.6632066999999999</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>1.8165528</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>1.9709994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-58B7-433A-9E91-5E8C457A562C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -890,6 +2265,7 @@
           <a:lumOff val="85000"/>
         </a:schemeClr>
       </a:solidFill>
+      <a:prstDash val="sysDot"/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -2069,6 +3445,159 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="Straight Connector 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{827B7F26-DA1B-467B-874A-A435BDD8179E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8046720" y="7452360"/>
+          <a:ext cx="7620" cy="1120140"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="Straight Connector 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4BB1F4E-FD23-475A-ACE9-3FC789B295EF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7734300" y="7452360"/>
+          <a:ext cx="320040" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>434340</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="Straight Connector 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5A5485B-C476-42D7-9C30-8104A5C7301F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7749540" y="8587740"/>
+          <a:ext cx="320040" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
       <xdr:row>1</xdr:row>
@@ -2691,6 +4220,1077 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7284720" y="5875020"/>
+          <a:ext cx="320040" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9524BBA0-7E4A-4FCD-8BC2-12AD2071AD33}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3009900" y="6172200"/>
+          <a:ext cx="7620" cy="1005840"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB422450-EF86-4546-860F-DF0C5C230A91}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6111240" y="6172200"/>
+          <a:ext cx="7620" cy="1005840"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Straight Connector 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33027954-2D08-43A7-902A-900203C916CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3025140" y="7178040"/>
+          <a:ext cx="320040" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Straight Connector 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACE72FD6-3C28-48BA-8E7F-51BF4718B67B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2994660" y="6172200"/>
+          <a:ext cx="320040" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Connector 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF87B2BF-98C1-41A3-BA41-F0BD17E67487}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5814060" y="7170420"/>
+          <a:ext cx="320040" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Straight Connector 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4146F8F1-C2AA-4F2A-B409-73A7678E0B75}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5814060" y="6187440"/>
+          <a:ext cx="320040" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>563880</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Straight Connector 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CADC810-4596-4566-8460-27D805D4985D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7269480" y="6019800"/>
+          <a:ext cx="15240" cy="1295400"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Straight Connector 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E548107-4AC1-433A-A7CE-6F99161158D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7947660" y="6027420"/>
+          <a:ext cx="22860" cy="1280160"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>281940</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Straight Connector 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A76F8C53-DE52-48AE-A34F-2A5CD4C203EB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7277100" y="6019800"/>
+          <a:ext cx="320040" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Straight Connector 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A44BAE51-049C-4763-AE45-8F52F788187D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7642860" y="6027420"/>
+          <a:ext cx="320040" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>350520</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Straight Connector 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B37E5B4F-E5A4-449A-A7E0-B569965E9BDE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7665720" y="7307580"/>
+          <a:ext cx="320040" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Straight Connector 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1083072E-A3D0-4244-8406-1F52F06CA330}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7284720" y="7315200"/>
+          <a:ext cx="320040" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="Straight Connector 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54CE4F5E-B9E6-49C2-85CB-E562F48E60E3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7284720" y="7459980"/>
+          <a:ext cx="15240" cy="1135380"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>281940</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="Straight Connector 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45370CFA-2D13-45C8-BA82-A97D1CDAC144}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7277100" y="7459980"/>
+          <a:ext cx="320040" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="Straight Connector 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81DEEDA4-CBF4-4CD1-8FD9-4109AE156038}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7284720" y="8595360"/>
+          <a:ext cx="320040" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="Straight Connector 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E9A4B72-5708-4C41-BA9D-86256962AEEB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7284720" y="8740140"/>
+          <a:ext cx="15240" cy="1150620"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Straight Connector 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C125300B-DD91-451E-8626-5E5C5BBF06E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8054340" y="8740140"/>
+          <a:ext cx="0" cy="1143000"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>281940</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="35" name="Straight Connector 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6887DFFF-3CEC-49F7-A8DC-CA7EF1CFD91E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7277100" y="8755380"/>
+          <a:ext cx="320040" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="Straight Connector 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C338895-BE29-4B79-B68E-3D3F4D7C6685}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7642860" y="8755380"/>
+          <a:ext cx="411480" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>350520</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="Straight Connector 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A8AF753-E463-4302-94A1-B6C57AF3D11F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7665720" y="9875520"/>
+          <a:ext cx="411480" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="38" name="Straight Connector 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A443243A-3A67-41D5-80DF-FB56B2D95C31}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7284720" y="9875520"/>
           <a:ext cx="320040" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -3037,17 +5637,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9784EF01-C92B-4A7D-A016-FBBD78E6DB83}">
   <dimension ref="B2:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6"/>
+      <c r="C2" s="7"/>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
@@ -3316,84 +5916,107 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FACAD2D-2FBB-4E4C-9746-35C411EA4F33}">
-  <dimension ref="B2:M34"/>
+  <dimension ref="B2:R144"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="77" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="P3" s="16"/>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="P4" s="16"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
         <v>-6</v>
       </c>
       <c r="C5" s="2">
         <v>2.5289999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="P5" s="16"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" s="2">
         <v>-4</v>
       </c>
       <c r="C6" s="2">
         <v>1.7569999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="P6" s="16"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" s="2">
         <v>-2</v>
       </c>
       <c r="C7" s="2">
         <v>-0.65900000000000003</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="P7" s="16"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8" s="2">
         <v>0</v>
       </c>
       <c r="C8" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="P8" s="16"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" s="2">
         <v>2</v>
       </c>
       <c r="C9" s="2">
         <v>1.159</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="P9" s="16"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" s="2">
         <v>4</v>
       </c>
       <c r="C10" s="2">
         <v>0.24299999999999999</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="P10" s="16"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B11" s="2">
         <v>6</v>
       </c>
       <c r="C11" s="2">
         <v>1.9710000000000001</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="P11" s="16"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="P12" s="16"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="P13" s="16"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="P14" s="16"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
         <v>4</v>
       </c>
@@ -3404,8 +6027,9 @@
       <c r="D15" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="P15" s="16"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B16" s="4" t="s">
         <v>5</v>
       </c>
@@ -3416,14 +6040,19 @@
       <c r="D16" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B18" s="7" t="s">
+      <c r="P16" s="16"/>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="P17" s="16"/>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B18" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="8"/>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C18" s="9"/>
+      <c r="P18" s="16"/>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B19" s="4" t="s">
         <v>9</v>
       </c>
@@ -3431,8 +6060,9 @@
         <f>B6-B5</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="P19" s="16"/>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B20" s="4" t="s">
         <v>10</v>
       </c>
@@ -3440,8 +6070,9 @@
         <f t="shared" ref="C20:C24" si="0">B7-B6</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="P20" s="16"/>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B21" s="4" t="s">
         <v>11</v>
       </c>
@@ -3449,8 +6080,9 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="P21" s="16"/>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B22" s="4" t="s">
         <v>12</v>
       </c>
@@ -3458,8 +6090,9 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="P22" s="16"/>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B23" s="4" t="s">
         <v>13</v>
       </c>
@@ -3467,8 +6100,9 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="P23" s="16"/>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B24" s="4" t="s">
         <v>14</v>
       </c>
@@ -3476,34 +6110,40 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B26" s="10" t="s">
+      <c r="P24" s="16"/>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="P25" s="16"/>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B26" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="10"/>
-      <c r="F26" s="10" t="s">
+      <c r="C26" s="11"/>
+      <c r="F26" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
-      <c r="M26" s="10"/>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B27" s="9" t="s">
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="P26" s="16"/>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B27" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="9"/>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C27" s="10"/>
+      <c r="P27" s="16"/>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B28" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="15">
         <f>C5</f>
         <v>2.5289999999999999</v>
       </c>
@@ -3524,16 +6164,17 @@
       <c r="J28" s="2">
         <v>0</v>
       </c>
-      <c r="M28" s="2">
+      <c r="M28" s="14">
         <f>(3/C20)*(C30-C29)-(3/C19)*(C29-C28)</f>
         <v>-2.4659999999999997</v>
       </c>
-    </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="P28" s="16"/>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="15">
         <f t="shared" ref="C29:C34" si="1">C6</f>
         <v>1.7569999999999999</v>
       </c>
@@ -3555,16 +6196,17 @@
       <c r="J29" s="2">
         <v>0</v>
       </c>
-      <c r="M29" s="2">
-        <f t="shared" ref="M29:M31" si="2">(3/C21)*(C31-C30)-(3/C20)*(C30-C29)</f>
+      <c r="M29" s="14">
+        <f>(3/C21)*(C31-C30)-(3/C20)*(C30-C29)</f>
         <v>4.6124999999999998</v>
       </c>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="P29" s="16"/>
+    </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B30" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30" s="15">
         <f t="shared" si="1"/>
         <v>-0.65900000000000003</v>
       </c>
@@ -3592,16 +6234,17 @@
       <c r="L30" t="s">
         <v>26</v>
       </c>
-      <c r="M30" s="2">
-        <f t="shared" si="2"/>
+      <c r="M30" s="14">
+        <f t="shared" ref="M29:M31" si="2">(3/C22)*(C32-C31)-(3/C21)*(C31-C30)</f>
         <v>0.75000000000000011</v>
       </c>
-    </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="P30" s="16"/>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B31" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C31" s="15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3623,16 +6266,19 @@
         <f>C23</f>
         <v>2</v>
       </c>
-      <c r="M31" s="2">
+      <c r="M31" s="14">
         <f t="shared" si="2"/>
         <v>-3.1125000000000003</v>
       </c>
-    </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="P31" s="16"/>
+      <c r="Q31" s="12"/>
+      <c r="R31" s="12"/>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B32" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="15">
         <f t="shared" si="1"/>
         <v>1.159</v>
       </c>
@@ -3653,35 +6299,1832 @@
         <f>2*(C23+C24)</f>
         <v>8</v>
       </c>
-      <c r="M32" s="2">
+      <c r="M32" s="14">
         <f>(3/C24)*(C34-C33)-(3/C23)*(C33-C32)</f>
         <v>3.9660000000000006</v>
       </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="P32" s="16"/>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B33" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="15">
         <f t="shared" si="1"/>
         <v>0.24299999999999999</v>
       </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="P33" s="16"/>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B34" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C34" s="15">
         <f t="shared" si="1"/>
         <v>1.9710000000000001</v>
       </c>
+      <c r="L34" t="s">
+        <v>31</v>
+      </c>
+      <c r="M34" s="13">
+        <v>0</v>
+      </c>
+      <c r="P34" s="16"/>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F35" s="13" cm="1">
+        <f t="array" ref="F35:J39">MINVERSE(F28:J32)</f>
+        <v>0.13397435897435897</v>
+      </c>
+      <c r="G35" s="13">
+        <v>-3.5897435897435895E-2</v>
+      </c>
+      <c r="H35" s="13">
+        <v>9.6153846153846142E-3</v>
+      </c>
+      <c r="I35" s="13">
+        <v>-2.5641025641025637E-3</v>
+      </c>
+      <c r="J35" s="13">
+        <v>6.4102564102564092E-4</v>
+      </c>
+      <c r="M35" s="13">
+        <f>($M$28*F35+$M$29*G35+$M$30*H35+$M$31*I35+$M$32*J35)</f>
+        <v>-0.47822307692307692</v>
+      </c>
+      <c r="P35" s="16"/>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F36" s="13">
+        <v>-3.5897435897435895E-2</v>
+      </c>
+      <c r="G36" s="13">
+        <v>0.14358974358974358</v>
+      </c>
+      <c r="H36" s="13">
+        <v>-3.8461538461538457E-2</v>
+      </c>
+      <c r="I36" s="13">
+        <v>1.0256410256410255E-2</v>
+      </c>
+      <c r="J36" s="13">
+        <v>-2.5641025641025637E-3</v>
+      </c>
+      <c r="M36" s="13">
+        <f>($M$28*F36+$M$29*G36+$M$30*H36+$M$31*I36+$M$32*J36)</f>
+        <v>0.67989230769230757</v>
+      </c>
+      <c r="P36" s="16"/>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="E37" t="s">
+        <v>27</v>
+      </c>
+      <c r="F37" s="13">
+        <v>9.6153846153846142E-3</v>
+      </c>
+      <c r="G37" s="13">
+        <v>-3.8461538461538457E-2</v>
+      </c>
+      <c r="H37" s="13">
+        <v>0.14423076923076922</v>
+      </c>
+      <c r="I37" s="13">
+        <v>-3.8461538461538457E-2</v>
+      </c>
+      <c r="J37" s="13">
+        <v>9.6153846153846142E-3</v>
+      </c>
+      <c r="L37" t="s">
+        <v>28</v>
+      </c>
+      <c r="M37" s="13">
+        <f>($M$28*F37+$M$29*G37+$M$30*H37+$M$31*I37+$M$32*J37)</f>
+        <v>6.4903846153846173E-2</v>
+      </c>
+      <c r="P37" s="16"/>
+    </row>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F38" s="13">
+        <v>-2.5641025641025637E-3</v>
+      </c>
+      <c r="G38" s="13">
+        <v>1.0256410256410255E-2</v>
+      </c>
+      <c r="H38" s="13">
+        <v>-3.8461538461538457E-2</v>
+      </c>
+      <c r="I38" s="13">
+        <v>0.14358974358974358</v>
+      </c>
+      <c r="J38" s="13">
+        <v>-3.5897435897435895E-2</v>
+      </c>
+      <c r="M38" s="13">
+        <f>($M$28*F38+$M$29*G38+$M$30*H38+$M$31*I38+$M$32*J38)</f>
+        <v>-0.56450769230769238</v>
+      </c>
+      <c r="P38" s="16"/>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F39" s="13">
+        <v>6.4102564102564103E-4</v>
+      </c>
+      <c r="G39" s="13">
+        <v>-2.5641025641025641E-3</v>
+      </c>
+      <c r="H39" s="13">
+        <v>9.6153846153846159E-3</v>
+      </c>
+      <c r="I39" s="13">
+        <v>-3.5897435897435902E-2</v>
+      </c>
+      <c r="J39" s="13">
+        <v>0.13397435897435897</v>
+      </c>
+      <c r="M39" s="13">
+        <f>($M$28*F39+$M$29*G39+$M$30*H39+$M$31*I39+$M$32*J39)</f>
+        <v>0.63687692307692312</v>
+      </c>
+      <c r="P39" s="16"/>
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="L40" t="s">
+        <v>32</v>
+      </c>
+      <c r="M40" s="13">
+        <v>0</v>
+      </c>
+      <c r="P40" s="16"/>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="P41" s="16"/>
+    </row>
+    <row r="42" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B42" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E42" s="11"/>
+      <c r="M42" s="13">
+        <f>((1/C19)*(C29-C28))-((C19/3)*(M35+2*M34))</f>
+        <v>-6.7184615384615398E-2</v>
+      </c>
+      <c r="P42" s="16"/>
+    </row>
+    <row r="43" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B43" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="M43" s="13">
+        <f t="shared" ref="M43:M47" si="3">((1/C20)*(C30-C29))-((C20/3)*(M36+2*M35))</f>
+        <v>-1.0236307692307691</v>
+      </c>
+      <c r="P43" s="16"/>
+    </row>
+    <row r="44" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B44" s="15">
+        <v>-6</v>
+      </c>
+      <c r="C44" s="15">
+        <f>$C$28+($M$42*(B44-$B$5))+($M$34*(B44-$B$5)^2)+($M$49*(B44-$B$5)^3)</f>
+        <v>2.5289999999999999</v>
+      </c>
+      <c r="D44" s="15">
+        <v>-6</v>
+      </c>
+      <c r="E44" s="15">
+        <v>2.5289999999999999</v>
+      </c>
+      <c r="L44" t="s">
+        <v>29</v>
+      </c>
+      <c r="M44" s="13">
+        <f t="shared" si="3"/>
+        <v>-0.62029230769230759</v>
+      </c>
+      <c r="P44" s="16"/>
+    </row>
+    <row r="45" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B45" s="15">
+        <v>-5.88</v>
+      </c>
+      <c r="C45" s="15">
+        <f t="shared" ref="C45:C60" si="4">$C$28+($M$42*(B45-$B$5))+($M$34*(B45-$B$5)^2)+($M$49*(B45-$B$5)^3)</f>
+        <v>2.5208001179076924</v>
+      </c>
+      <c r="D45" s="15">
+        <v>-5.88</v>
+      </c>
+      <c r="E45" s="15">
+        <v>2.5208001000000002</v>
+      </c>
+      <c r="M45" s="13">
+        <f t="shared" si="3"/>
+        <v>0.86929999999999996</v>
+      </c>
+      <c r="P45" s="16"/>
+    </row>
+    <row r="46" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B46" s="15">
+        <v>-5.76</v>
+      </c>
+      <c r="C46" s="15">
+        <f t="shared" si="4"/>
+        <v>2.5117738663384617</v>
+      </c>
+      <c r="D46" s="15">
+        <v>-5.76</v>
+      </c>
+      <c r="E46" s="15">
+        <v>2.5117737999999998</v>
+      </c>
+      <c r="M46" s="13">
+        <f t="shared" si="3"/>
+        <v>-0.12990769230769228</v>
+      </c>
+      <c r="P46" s="16"/>
+    </row>
+    <row r="47" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B47" s="15">
+        <v>-5.64</v>
+      </c>
+      <c r="C47" s="15">
+        <f t="shared" si="4"/>
+        <v>2.5010948758153844</v>
+      </c>
+      <c r="D47" s="15">
+        <v>-5.64</v>
+      </c>
+      <c r="E47" s="15">
+        <v>2.5010948000000002</v>
+      </c>
+      <c r="M47" s="13">
+        <f t="shared" si="3"/>
+        <v>1.4830769230769314E-2</v>
+      </c>
+      <c r="P47" s="16"/>
+    </row>
+    <row r="48" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B48" s="15">
+        <v>-5.52</v>
+      </c>
+      <c r="C48" s="15">
+        <f t="shared" si="4"/>
+        <v>2.4879367768615386</v>
+      </c>
+      <c r="D48" s="15">
+        <v>-5.52</v>
+      </c>
+      <c r="E48" s="15">
+        <v>2.4879367000000001</v>
+      </c>
+      <c r="P48" s="16"/>
+    </row>
+    <row r="49" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B49" s="15">
+        <v>-5.3999999999999995</v>
+      </c>
+      <c r="C49" s="15">
+        <f t="shared" si="4"/>
+        <v>2.4714732000000001</v>
+      </c>
+      <c r="D49" s="15">
+        <v>-5.3999999999999995</v>
+      </c>
+      <c r="E49" s="15">
+        <v>2.4714732000000001</v>
+      </c>
+      <c r="M49" s="13">
+        <f>(1/(3*C19))*(M35-M34)</f>
+        <v>-7.9703846153846153E-2</v>
+      </c>
+      <c r="P49" s="16"/>
+    </row>
+    <row r="50" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B50" s="15">
+        <v>-5.2799999999999994</v>
+      </c>
+      <c r="C50" s="15">
+        <f t="shared" si="4"/>
+        <v>2.4508777757538462</v>
+      </c>
+      <c r="D50" s="15">
+        <v>-5.2799999999999994</v>
+      </c>
+      <c r="E50" s="15">
+        <v>2.4508779000000001</v>
+      </c>
+      <c r="M50" s="13">
+        <f t="shared" ref="M50:M54" si="5">(1/(3*C20))*(M36-M35)</f>
+        <v>0.19301923076923072</v>
+      </c>
+      <c r="P50" s="16"/>
+    </row>
+    <row r="51" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B51" s="15">
+        <v>-5.1599999999999993</v>
+      </c>
+      <c r="C51" s="15">
+        <f t="shared" si="4"/>
+        <v>2.4253241346461536</v>
+      </c>
+      <c r="D51" s="15">
+        <v>-5.1599999999999993</v>
+      </c>
+      <c r="E51" s="15">
+        <v>2.4253241999999999</v>
+      </c>
+      <c r="L51" t="s">
+        <v>30</v>
+      </c>
+      <c r="M51" s="13">
+        <f t="shared" si="5"/>
+        <v>-0.1024980769230769</v>
+      </c>
+      <c r="P51" s="16"/>
+    </row>
+    <row r="52" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B52" s="15">
+        <v>-5.0399999999999991</v>
+      </c>
+      <c r="C52" s="15">
+        <f t="shared" si="4"/>
+        <v>2.3939859071999998</v>
+      </c>
+      <c r="D52" s="15">
+        <v>-5.0399999999999991</v>
+      </c>
+      <c r="E52" s="15">
+        <v>2.3939859999999999</v>
+      </c>
+      <c r="M52" s="13">
+        <f t="shared" si="5"/>
+        <v>-0.10490192307692309</v>
+      </c>
+      <c r="P52" s="16"/>
+    </row>
+    <row r="53" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B53" s="15">
+        <v>-4.919999999999999</v>
+      </c>
+      <c r="C53" s="15">
+        <f t="shared" si="4"/>
+        <v>2.3560367239384608</v>
+      </c>
+      <c r="D53" s="15">
+        <v>-4.919999999999999</v>
+      </c>
+      <c r="E53" s="15">
+        <v>2.3560367000000002</v>
+      </c>
+      <c r="M53" s="13">
+        <f t="shared" si="5"/>
+        <v>0.20023076923076924</v>
+      </c>
+      <c r="P53" s="16"/>
+      <c r="Q53" s="12"/>
+      <c r="R53" s="12"/>
+    </row>
+    <row r="54" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B54" s="15">
+        <v>-4.7999999999999989</v>
+      </c>
+      <c r="C54" s="15">
+        <f t="shared" si="4"/>
+        <v>2.3106502153846145</v>
+      </c>
+      <c r="D54" s="15">
+        <v>-4.7999999999999989</v>
+      </c>
+      <c r="E54" s="15">
+        <v>2.3106502999999998</v>
+      </c>
+      <c r="M54" s="13">
+        <f t="shared" si="5"/>
+        <v>-0.10614615384615385</v>
+      </c>
+      <c r="P54" s="16"/>
+    </row>
+    <row r="55" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B55" s="15">
+        <v>-4.6799999999999988</v>
+      </c>
+      <c r="C55" s="15">
+        <f t="shared" si="4"/>
+        <v>2.2570000120615377</v>
+      </c>
+      <c r="D55" s="15">
+        <v>-4.6799999999999988</v>
+      </c>
+      <c r="E55" s="15">
+        <v>2.2570000000000001</v>
+      </c>
+      <c r="P55" s="16"/>
+    </row>
+    <row r="56" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B56" s="15">
+        <v>-4.5599999999999987</v>
+      </c>
+      <c r="C56" s="15">
+        <f t="shared" si="4"/>
+        <v>2.1942597444923067</v>
+      </c>
+      <c r="D56" s="15">
+        <v>-4.5599999999999987</v>
+      </c>
+      <c r="E56" s="15">
+        <v>2.1942596000000001</v>
+      </c>
+      <c r="P56" s="16"/>
+    </row>
+    <row r="57" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B57" s="15">
+        <v>-4.4399999999999986</v>
+      </c>
+      <c r="C57" s="15">
+        <f t="shared" si="4"/>
+        <v>2.121603043199999</v>
+      </c>
+      <c r="D57" s="15">
+        <v>-4.4399999999999986</v>
+      </c>
+      <c r="E57" s="15">
+        <v>2.1216029999999999</v>
+      </c>
+      <c r="P57" s="16"/>
+    </row>
+    <row r="58" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B58" s="15">
+        <v>-4.3199999999999985</v>
+      </c>
+      <c r="C58" s="15">
+        <f t="shared" si="4"/>
+        <v>2.0382035387076911</v>
+      </c>
+      <c r="D58" s="15">
+        <v>-4.3199999999999985</v>
+      </c>
+      <c r="E58" s="15">
+        <v>2.0382037</v>
+      </c>
+      <c r="P58" s="16"/>
+    </row>
+    <row r="59" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B59" s="15">
+        <v>-4.1999999999999984</v>
+      </c>
+      <c r="C59" s="15">
+        <f t="shared" si="4"/>
+        <v>1.94323486153846</v>
+      </c>
+      <c r="D59" s="15">
+        <v>-4.1999999999999984</v>
+      </c>
+      <c r="E59" s="15">
+        <v>1.9432347000000001</v>
+      </c>
+      <c r="P59" s="16"/>
+    </row>
+    <row r="60" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B60" s="15">
+        <v>-4.0799999999999983</v>
+      </c>
+      <c r="C60" s="15">
+        <f t="shared" si="4"/>
+        <v>1.8358706422153828</v>
+      </c>
+      <c r="D60" s="15">
+        <v>-4.0799999999999983</v>
+      </c>
+      <c r="E60" s="15">
+        <v>1.8358705</v>
+      </c>
+      <c r="P60" s="16"/>
+    </row>
+    <row r="61" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B61" s="15">
+        <v>-3.9599999999999982</v>
+      </c>
+      <c r="C61" s="15">
+        <f>$C$29+($M$43*(B61-$B$6))+($M$35*(B61-$B$6)^2)+($M$50*(B61-$B$6)^3)</f>
+        <v>1.7153019655384596</v>
+      </c>
+      <c r="D61" s="15">
+        <v>-3.9599999999999982</v>
+      </c>
+      <c r="E61" s="15">
+        <v>1.7153020000000001</v>
+      </c>
+      <c r="P61" s="16"/>
+    </row>
+    <row r="62" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B62" s="15">
+        <v>-3.8399999999999981</v>
+      </c>
+      <c r="C62" s="15">
+        <f t="shared" ref="C62:C78" si="6">$C$29+($M$43*(B62-$B$6))+($M$35*(B62-$B$6)^2)+($M$50*(B62-$B$6)^3)</f>
+        <v>1.5817671729230747</v>
+      </c>
+      <c r="D62" s="15">
+        <v>-3.8399999999999981</v>
+      </c>
+      <c r="E62" s="15">
+        <v>1.5817673000000001</v>
+      </c>
+      <c r="P62" s="16"/>
+    </row>
+    <row r="63" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B63" s="15">
+        <v>-3.719999999999998</v>
+      </c>
+      <c r="C63" s="15">
+        <f t="shared" si="6"/>
+        <v>1.4371278535384588</v>
+      </c>
+      <c r="D63" s="15">
+        <v>-3.719999999999998</v>
+      </c>
+      <c r="E63" s="15">
+        <v>1.4371278000000001</v>
+      </c>
+      <c r="P63" s="16"/>
+    </row>
+    <row r="64" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B64" s="15">
+        <v>-3.5999999999999979</v>
+      </c>
+      <c r="C64" s="15">
+        <f t="shared" si="6"/>
+        <v>1.2833852307692279</v>
+      </c>
+      <c r="D64" s="15">
+        <v>-3.5999999999999979</v>
+      </c>
+      <c r="E64" s="15">
+        <v>1.2833854</v>
+      </c>
+      <c r="P64" s="16"/>
+    </row>
+    <row r="65" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B65" s="15">
+        <v>-3.4799999999999978</v>
+      </c>
+      <c r="C65" s="15">
+        <f t="shared" si="6"/>
+        <v>1.1225405279999969</v>
+      </c>
+      <c r="D65" s="15">
+        <v>-3.4799999999999978</v>
+      </c>
+      <c r="E65" s="15">
+        <v>1.1225404999999999</v>
+      </c>
+      <c r="P65" s="16"/>
+    </row>
+    <row r="66" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B66" s="15">
+        <v>-3.3599999999999977</v>
+      </c>
+      <c r="C66" s="15">
+        <f t="shared" si="6"/>
+        <v>0.95659496861538129</v>
+      </c>
+      <c r="D66" s="15">
+        <v>-3.3599999999999977</v>
+      </c>
+      <c r="E66" s="15">
+        <v>0.95659506000000005</v>
+      </c>
+      <c r="P66" s="16"/>
+    </row>
+    <row r="67" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B67" s="15">
+        <v>-3.2399999999999975</v>
+      </c>
+      <c r="C67" s="15">
+        <f t="shared" si="6"/>
+        <v>0.78754977599999643</v>
+      </c>
+      <c r="D67" s="15">
+        <v>-3.2399999999999975</v>
+      </c>
+      <c r="E67" s="15">
+        <v>0.78754972999999995</v>
+      </c>
+      <c r="P67" s="16"/>
+    </row>
+    <row r="68" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B68" s="15">
+        <v>-3.1199999999999974</v>
+      </c>
+      <c r="C68" s="15">
+        <f t="shared" si="6"/>
+        <v>0.61740617353845784</v>
+      </c>
+      <c r="D68" s="15">
+        <v>-3.1199999999999974</v>
+      </c>
+      <c r="E68" s="15">
+        <v>0.61740625000000005</v>
+      </c>
+      <c r="P68" s="16"/>
+    </row>
+    <row r="69" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B69" s="15">
+        <v>-2.9999999999999973</v>
+      </c>
+      <c r="C69" s="15">
+        <f t="shared" si="6"/>
+        <v>0.44816538461538091</v>
+      </c>
+      <c r="D69" s="15">
+        <v>-2.9999999999999973</v>
+      </c>
+      <c r="E69" s="15">
+        <v>0.44816529999999999</v>
+      </c>
+      <c r="P69" s="16"/>
+    </row>
+    <row r="70" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B70" s="15">
+        <v>-2.8799999999999972</v>
+      </c>
+      <c r="C70" s="15">
+        <f t="shared" si="6"/>
+        <v>0.28182863261538077</v>
+      </c>
+      <c r="D70" s="15">
+        <v>-2.8799999999999972</v>
+      </c>
+      <c r="E70" s="15">
+        <v>0.28182869999999999</v>
+      </c>
+      <c r="P70" s="16"/>
+    </row>
+    <row r="71" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B71" s="15">
+        <v>-2.7599999999999971</v>
+      </c>
+      <c r="C71" s="15">
+        <f t="shared" si="6"/>
+        <v>0.12039714092307313</v>
+      </c>
+      <c r="D71" s="15">
+        <v>-2.7599999999999971</v>
+      </c>
+      <c r="E71" s="15">
+        <v>0.12039704</v>
+      </c>
+      <c r="P71" s="16"/>
+    </row>
+    <row r="72" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B72" s="15">
+        <v>-2.639999999999997</v>
+      </c>
+      <c r="C72" s="15">
+        <f t="shared" si="6"/>
+        <v>-3.4127867076926943E-2</v>
+      </c>
+      <c r="D72" s="15">
+        <v>-2.639999999999997</v>
+      </c>
+      <c r="E72" s="15">
+        <v>-3.41278203E-2</v>
+      </c>
+      <c r="P72" s="16"/>
+    </row>
+    <row r="73" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B73" s="15">
+        <v>-2.5199999999999969</v>
+      </c>
+      <c r="C73" s="15">
+        <f t="shared" si="6"/>
+        <v>-0.17974516800000384</v>
+      </c>
+      <c r="D73" s="15">
+        <v>-2.5199999999999969</v>
+      </c>
+      <c r="E73" s="15">
+        <v>-0.17974527000000001</v>
+      </c>
+      <c r="P73" s="16"/>
+    </row>
+    <row r="74" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B74" s="15">
+        <v>-2.3999999999999968</v>
+      </c>
+      <c r="C74" s="15">
+        <f t="shared" si="6"/>
+        <v>-0.31445353846154189</v>
+      </c>
+      <c r="D74" s="15">
+        <v>-2.3999999999999968</v>
+      </c>
+      <c r="E74" s="15">
+        <v>-0.31445350999999999</v>
+      </c>
+      <c r="P74" s="16"/>
+    </row>
+    <row r="75" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B75" s="15">
+        <v>-2.2799999999999967</v>
+      </c>
+      <c r="C75" s="15">
+        <f t="shared" si="6"/>
+        <v>-0.43625175507692637</v>
+      </c>
+      <c r="D75" s="15">
+        <v>-2.2799999999999967</v>
+      </c>
+      <c r="E75" s="15">
+        <v>-0.43625185</v>
+      </c>
+      <c r="P75" s="16"/>
+    </row>
+    <row r="76" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B76" s="15">
+        <v>-2.1599999999999966</v>
+      </c>
+      <c r="C76" s="15">
+        <f t="shared" si="6"/>
+        <v>-0.54313859446154145</v>
+      </c>
+      <c r="D76" s="15">
+        <v>-2.1599999999999966</v>
+      </c>
+      <c r="E76" s="15">
+        <v>-0.54313856000000005</v>
+      </c>
+      <c r="P76" s="16"/>
+    </row>
+    <row r="77" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B77" s="15">
+        <v>-2.0399999999999965</v>
+      </c>
+      <c r="C77" s="15">
+        <f t="shared" si="6"/>
+        <v>-0.63311283323077228</v>
+      </c>
+      <c r="D77" s="15">
+        <v>-2.0399999999999965</v>
+      </c>
+      <c r="E77" s="15">
+        <v>-0.63311273000000001</v>
+      </c>
+      <c r="P77" s="16"/>
+    </row>
+    <row r="78" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B78" s="15">
+        <v>-1.9199999999999964</v>
+      </c>
+      <c r="C78" s="15">
+        <f>$C$30+($M$44*(B78-$B$7))+($M$36*(B78-$B$7)^2)+($M$51*(B78-$B$7)^3)</f>
+        <v>-0.70432455286154039</v>
+      </c>
+      <c r="D78" s="15">
+        <v>-1.9199999999999964</v>
+      </c>
+      <c r="E78" s="15">
+        <v>-0.70432448000000003</v>
+      </c>
+      <c r="P78" s="16"/>
+    </row>
+    <row r="79" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B79" s="15">
+        <v>-1.7999999999999963</v>
+      </c>
+      <c r="C79" s="15">
+        <f t="shared" ref="C79:C94" si="7">$C$30+($M$44*(B79-$B$7))+($M$36*(B79-$B$7)^2)+($M$51*(B79-$B$7)^3)</f>
+        <v>-0.75668275384615524</v>
+      </c>
+      <c r="D79" s="15">
+        <v>-1.7999999999999963</v>
+      </c>
+      <c r="E79" s="15">
+        <v>-0.75668274999999996</v>
+      </c>
+      <c r="P79" s="16"/>
+    </row>
+    <row r="80" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B80" s="15">
+        <v>-1.6799999999999962</v>
+      </c>
+      <c r="C80" s="15">
+        <f t="shared" si="7"/>
+        <v>-0.79123122313846239</v>
+      </c>
+      <c r="D80" s="15">
+        <v>-1.6799999999999962</v>
+      </c>
+      <c r="E80" s="15">
+        <v>-0.79123122000000001</v>
+      </c>
+      <c r="P80" s="16"/>
+    </row>
+    <row r="81" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B81" s="15">
+        <v>-1.5599999999999961</v>
+      </c>
+      <c r="C81" s="15">
+        <f t="shared" si="7"/>
+        <v>-0.80903266080000036</v>
+      </c>
+      <c r="D81" s="15">
+        <v>-1.5599999999999961</v>
+      </c>
+      <c r="E81" s="15">
+        <v>-0.80903267999999995</v>
+      </c>
+      <c r="P81" s="16"/>
+    </row>
+    <row r="82" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B82" s="15">
+        <v>-1.4399999999999959</v>
+      </c>
+      <c r="C82" s="15">
+        <f t="shared" si="7"/>
+        <v>-0.81114976689230756</v>
+      </c>
+      <c r="D82" s="15">
+        <v>-1.4399999999999959</v>
+      </c>
+      <c r="E82" s="15">
+        <v>-0.81114978000000004</v>
+      </c>
+      <c r="P82" s="16"/>
+    </row>
+    <row r="83" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B83" s="15">
+        <v>-1.3199999999999958</v>
+      </c>
+      <c r="C83" s="15">
+        <f t="shared" si="7"/>
+        <v>-0.79864524147692229</v>
+      </c>
+      <c r="D83" s="15">
+        <v>-1.3199999999999958</v>
+      </c>
+      <c r="E83" s="15">
+        <v>-0.79864526000000002</v>
+      </c>
+      <c r="P83" s="16"/>
+    </row>
+    <row r="84" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B84" s="15">
+        <v>-1.1999999999999957</v>
+      </c>
+      <c r="C84" s="15">
+        <f t="shared" si="7"/>
+        <v>-0.77258178461538352</v>
+      </c>
+      <c r="D84" s="15">
+        <v>-1.1999999999999957</v>
+      </c>
+      <c r="E84" s="15">
+        <v>-0.77258181999999997</v>
+      </c>
+      <c r="P84" s="16"/>
+    </row>
+    <row r="85" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B85" s="15">
+        <v>-1.0799999999999956</v>
+      </c>
+      <c r="C85" s="15">
+        <f t="shared" si="7"/>
+        <v>-0.73402209636922922</v>
+      </c>
+      <c r="D85" s="15">
+        <v>-1.0799999999999956</v>
+      </c>
+      <c r="E85" s="15">
+        <v>-0.73402219999999996</v>
+      </c>
+      <c r="P85" s="16"/>
+    </row>
+    <row r="86" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B86" s="15">
+        <v>-0.95999999999999563</v>
+      </c>
+      <c r="C86" s="15">
+        <f t="shared" si="7"/>
+        <v>-0.68402887679999813</v>
+      </c>
+      <c r="D86" s="15">
+        <v>-0.95999999999999563</v>
+      </c>
+      <c r="E86" s="15">
+        <v>-0.68402898000000001</v>
+      </c>
+      <c r="P86" s="16"/>
+    </row>
+    <row r="87" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B87" s="15">
+        <v>-0.83999999999999564</v>
+      </c>
+      <c r="C87" s="15">
+        <f t="shared" si="7"/>
+        <v>-0.62366482596922834</v>
+      </c>
+      <c r="D87" s="15">
+        <v>-0.83999999999999564</v>
+      </c>
+      <c r="E87" s="15">
+        <v>-0.62366491999999996</v>
+      </c>
+      <c r="P87" s="16"/>
+    </row>
+    <row r="88" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B88" s="15">
+        <v>-0.71999999999999564</v>
+      </c>
+      <c r="C88" s="15">
+        <f t="shared" si="7"/>
+        <v>-0.55399264393845893</v>
+      </c>
+      <c r="D88" s="15">
+        <v>-0.71999999999999564</v>
+      </c>
+      <c r="E88" s="15">
+        <v>-0.55399281</v>
+      </c>
+      <c r="P88" s="16"/>
+    </row>
+    <row r="89" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B89" s="15">
+        <v>-0.59999999999999565</v>
+      </c>
+      <c r="C89" s="15">
+        <f t="shared" si="7"/>
+        <v>-0.47607503076922791</v>
+      </c>
+      <c r="D89" s="15">
+        <v>-0.59999999999999565</v>
+      </c>
+      <c r="E89" s="15">
+        <v>-0.47607519999999998</v>
+      </c>
+      <c r="P89" s="16"/>
+    </row>
+    <row r="90" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B90" s="15">
+        <v>-0.47999999999999565</v>
+      </c>
+      <c r="C90" s="15">
+        <f t="shared" si="7"/>
+        <v>-0.39097468652307354</v>
+      </c>
+      <c r="D90" s="15">
+        <v>-0.47999999999999565</v>
+      </c>
+      <c r="E90" s="15">
+        <v>-0.39097484999999998</v>
+      </c>
+      <c r="P90" s="16"/>
+    </row>
+    <row r="91" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B91" s="15">
+        <v>-0.35999999999999566</v>
+      </c>
+      <c r="C91" s="15">
+        <f t="shared" si="7"/>
+        <v>-0.29975431126153523</v>
+      </c>
+      <c r="D91" s="15">
+        <v>-0.35999999999999566</v>
+      </c>
+      <c r="E91" s="15">
+        <v>-0.29975447</v>
+      </c>
+      <c r="P91" s="16"/>
+    </row>
+    <row r="92" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B92" s="15">
+        <v>-0.23999999999999566</v>
+      </c>
+      <c r="C92" s="15">
+        <f t="shared" si="7"/>
+        <v>-0.20347660504615062</v>
+      </c>
+      <c r="D92" s="15">
+        <v>-0.23999999999999566</v>
+      </c>
+      <c r="E92" s="15">
+        <v>-0.20347677</v>
+      </c>
+      <c r="P92" s="16"/>
+    </row>
+    <row r="93" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B93" s="15">
+        <v>-0.11999999999999567</v>
+      </c>
+      <c r="C93" s="15">
+        <f t="shared" si="7"/>
+        <v>-0.10320426793845783</v>
+      </c>
+      <c r="D93" s="15">
+        <v>-0.11999999999999567</v>
+      </c>
+      <c r="E93" s="15">
+        <v>-0.10320443999999999</v>
+      </c>
+      <c r="P93" s="16"/>
+    </row>
+    <row r="94" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B94" s="15">
+        <v>4.3298697960381105E-15</v>
+      </c>
+      <c r="C94" s="15">
+        <f>$C$31+($M$45*(B94-$B$8))+($M$37*(B94-$B$8)^2)+($M$52*(B94-$B$8)^3)</f>
+        <v>3.7639558136959306E-15</v>
+      </c>
+      <c r="D94" s="15">
+        <v>4.3298697960381105E-15</v>
+      </c>
+      <c r="E94" s="15">
+        <v>-1.7618685900000001E-7</v>
+      </c>
+      <c r="P94" s="16"/>
+    </row>
+    <row r="95" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B95" s="15">
+        <v>0.12000000000000433</v>
+      </c>
+      <c r="C95" s="15">
+        <f t="shared" ref="C95:C111" si="8">$C$31+($M$45*(B95-$B$8))+($M$37*(B95-$B$8)^2)+($M$52*(B95-$B$8)^3)</f>
+        <v>0.10506934486154226</v>
+      </c>
+      <c r="D95" s="15">
+        <v>0.12000000000000433</v>
+      </c>
+      <c r="E95" s="15">
+        <v>0.10506923</v>
+      </c>
+      <c r="P95" s="16"/>
+    </row>
+    <row r="96" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B96" s="15">
+        <v>0.24000000000000432</v>
+      </c>
+      <c r="C96" s="15">
+        <f t="shared" si="8"/>
+        <v>0.21092029735384996</v>
+      </c>
+      <c r="D96" s="15">
+        <v>0.24000000000000432</v>
+      </c>
+      <c r="E96" s="15">
+        <v>0.21092018000000001</v>
+      </c>
+      <c r="P96" s="16"/>
+    </row>
+    <row r="97" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B97" s="15">
+        <v>0.36000000000000432</v>
+      </c>
+      <c r="C97" s="15">
+        <f t="shared" si="8"/>
+        <v>0.3164652343384653</v>
+      </c>
+      <c r="D97" s="15">
+        <v>0.36000000000000432</v>
+      </c>
+      <c r="E97" s="15">
+        <v>0.31646510999999999</v>
+      </c>
+      <c r="P97" s="16"/>
+    </row>
+    <row r="98" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B98" s="15">
+        <v>0.48000000000000431</v>
+      </c>
+      <c r="C98" s="15">
+        <f t="shared" si="8"/>
+        <v>0.42061653267692678</v>
+      </c>
+      <c r="D98" s="15">
+        <v>0.48000000000000431</v>
+      </c>
+      <c r="E98" s="15">
+        <v>0.42061641999999999</v>
+      </c>
+      <c r="P98" s="16"/>
+    </row>
+    <row r="99" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B99" s="15">
+        <v>0.60000000000000431</v>
+      </c>
+      <c r="C99" s="15">
+        <f t="shared" si="8"/>
+        <v>0.52228656923077277</v>
+      </c>
+      <c r="D99" s="15">
+        <v>0.60000000000000431</v>
+      </c>
+      <c r="E99" s="15">
+        <v>0.52228646999999995</v>
+      </c>
+      <c r="P99" s="16"/>
+    </row>
+    <row r="100" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B100" s="15">
+        <v>0.7200000000000043</v>
+      </c>
+      <c r="C100" s="15">
+        <f t="shared" si="8"/>
+        <v>0.62038772086154181</v>
+      </c>
+      <c r="D100" s="15">
+        <v>0.7200000000000043</v>
+      </c>
+      <c r="E100" s="15">
+        <v>0.62038760999999998</v>
+      </c>
+      <c r="P100" s="16"/>
+    </row>
+    <row r="101" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B101" s="15">
+        <v>0.8400000000000043</v>
+      </c>
+      <c r="C101" s="15">
+        <f t="shared" si="8"/>
+        <v>0.71383236443077247</v>
+      </c>
+      <c r="D101" s="15">
+        <v>0.8400000000000043</v>
+      </c>
+      <c r="E101" s="15">
+        <v>0.71383226</v>
+      </c>
+      <c r="P101" s="16"/>
+    </row>
+    <row r="102" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B102" s="15">
+        <v>0.96000000000000429</v>
+      </c>
+      <c r="C102" s="15">
+        <f t="shared" si="8"/>
+        <v>0.80153287680000296</v>
+      </c>
+      <c r="D102" s="15">
+        <v>0.96000000000000429</v>
+      </c>
+      <c r="E102" s="15">
+        <v>0.80153280000000005</v>
+      </c>
+      <c r="P102" s="16"/>
+    </row>
+    <row r="103" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B103" s="15">
+        <v>1.0800000000000043</v>
+      </c>
+      <c r="C103" s="15">
+        <f t="shared" si="8"/>
+        <v>0.88240163483077194</v>
+      </c>
+      <c r="D103" s="15">
+        <v>1.0800000000000043</v>
+      </c>
+      <c r="E103" s="15">
+        <v>0.88240152999999999</v>
+      </c>
+      <c r="P103" s="16"/>
+    </row>
+    <row r="104" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B104" s="15">
+        <v>1.2000000000000042</v>
+      </c>
+      <c r="C104" s="15">
+        <f t="shared" si="8"/>
+        <v>0.95535101538461786</v>
+      </c>
+      <c r="D104" s="15">
+        <v>1.2000000000000042</v>
+      </c>
+      <c r="E104" s="15">
+        <v>0.95535093999999998</v>
+      </c>
+    </row>
+    <row r="105" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B105" s="15">
+        <v>1.3200000000000043</v>
+      </c>
+      <c r="C105" s="15">
+        <f t="shared" si="8"/>
+        <v>1.0192933953230792</v>
+      </c>
+      <c r="D105" s="15">
+        <v>1.3200000000000043</v>
+      </c>
+      <c r="E105" s="15">
+        <v>1.0192933</v>
+      </c>
+    </row>
+    <row r="106" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B106" s="15">
+        <v>1.4400000000000044</v>
+      </c>
+      <c r="C106" s="15">
+        <f t="shared" si="8"/>
+        <v>1.0731411515076941</v>
+      </c>
+      <c r="D106" s="15">
+        <v>1.4400000000000044</v>
+      </c>
+      <c r="E106" s="15">
+        <v>1.0731411</v>
+      </c>
+    </row>
+    <row r="107" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B107" s="15">
+        <v>1.5600000000000045</v>
+      </c>
+      <c r="C107" s="15">
+        <f t="shared" si="8"/>
+        <v>1.1158066608000015</v>
+      </c>
+      <c r="D107" s="15">
+        <v>1.5600000000000045</v>
+      </c>
+      <c r="E107" s="15">
+        <v>1.1158067</v>
+      </c>
+    </row>
+    <row r="108" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B108" s="15">
+        <v>1.6800000000000046</v>
+      </c>
+      <c r="C108" s="15">
+        <f t="shared" si="8"/>
+        <v>1.1462023000615393</v>
+      </c>
+      <c r="D108" s="15">
+        <v>1.6800000000000046</v>
+      </c>
+      <c r="E108" s="15">
+        <v>1.1462022999999999</v>
+      </c>
+    </row>
+    <row r="109" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B109" s="15">
+        <v>1.8000000000000047</v>
+      </c>
+      <c r="C109" s="15">
+        <f t="shared" si="8"/>
+        <v>1.1632404461538466</v>
+      </c>
+      <c r="D109" s="15">
+        <v>1.8000000000000047</v>
+      </c>
+      <c r="E109" s="15">
+        <v>1.1632406</v>
+      </c>
+    </row>
+    <row r="110" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B110" s="15">
+        <v>1.9200000000000048</v>
+      </c>
+      <c r="C110" s="15">
+        <f t="shared" si="8"/>
+        <v>1.1658334759384612</v>
+      </c>
+      <c r="D110" s="15">
+        <v>1.9200000000000048</v>
+      </c>
+      <c r="E110" s="15">
+        <v>1.1658336</v>
+      </c>
+    </row>
+    <row r="111" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B111" s="15">
+        <v>2.0400000000000049</v>
+      </c>
+      <c r="C111" s="15">
+        <f>$C$32+($M$46*(B111-$B$9))+($M$38*(B111-$B$9)^2)+($M$53*(B111-$B$9)^3)</f>
+        <v>1.15291329476923</v>
+      </c>
+      <c r="D111" s="15">
+        <v>2.0400000000000049</v>
+      </c>
+      <c r="E111" s="15">
+        <v>1.1529133</v>
+      </c>
+    </row>
+    <row r="112" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B112" s="15">
+        <v>2.160000000000005</v>
+      </c>
+      <c r="C112" s="15">
+        <f t="shared" ref="C112:C128" si="9">$C$32+($M$46*(B112-$B$9))+($M$38*(B112-$B$9)^2)+($M$53*(B112-$B$9)^3)</f>
+        <v>1.1245835175384602</v>
+      </c>
+      <c r="D112" s="15">
+        <v>2.160000000000005</v>
+      </c>
+      <c r="E112" s="15">
+        <v>1.1245836</v>
+      </c>
+    </row>
+    <row r="113" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B113" s="15">
+        <v>2.2800000000000051</v>
+      </c>
+      <c r="C113" s="15">
+        <f t="shared" si="9"/>
+        <v>1.0827639089230747</v>
+      </c>
+      <c r="D113" s="15">
+        <v>2.2800000000000051</v>
+      </c>
+      <c r="E113" s="15">
+        <v>1.0827640000000001</v>
+      </c>
+    </row>
+    <row r="114" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B114" s="15">
+        <v>2.4000000000000052</v>
+      </c>
+      <c r="C114" s="15">
+        <f t="shared" si="9"/>
+        <v>1.0295304615384588</v>
+      </c>
+      <c r="D114" s="15">
+        <v>2.4000000000000052</v>
+      </c>
+      <c r="E114" s="15">
+        <v>1.0295304999999999</v>
+      </c>
+    </row>
+    <row r="115" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B115" s="15">
+        <v>2.5200000000000053</v>
+      </c>
+      <c r="C115" s="15">
+        <f t="shared" si="9"/>
+        <v>0.96695916799999704</v>
+      </c>
+      <c r="D115" s="15">
+        <v>2.5200000000000053</v>
+      </c>
+      <c r="E115" s="15">
+        <v>0.96695936000000005</v>
+      </c>
+    </row>
+    <row r="116" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B116" s="15">
+        <v>2.6400000000000055</v>
+      </c>
+      <c r="C116" s="15">
+        <f t="shared" si="9"/>
+        <v>0.8971260209230737</v>
+      </c>
+      <c r="D116" s="15">
+        <v>2.6400000000000055</v>
+      </c>
+      <c r="E116" s="15">
+        <v>0.89712614000000002</v>
+      </c>
+    </row>
+    <row r="117" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B117" s="15">
+        <v>2.7600000000000056</v>
+      </c>
+      <c r="C117" s="15">
+        <f t="shared" si="9"/>
+        <v>0.82210701292307342</v>
+      </c>
+      <c r="D117" s="15">
+        <v>2.7600000000000056</v>
+      </c>
+      <c r="E117" s="15">
+        <v>0.82210720000000004</v>
+      </c>
+    </row>
+    <row r="118" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B118" s="15">
+        <v>2.8800000000000057</v>
+      </c>
+      <c r="C118" s="15">
+        <f t="shared" si="9"/>
+        <v>0.74397813661538093</v>
+      </c>
+      <c r="D118" s="15">
+        <v>2.8800000000000057</v>
+      </c>
+      <c r="E118" s="15">
+        <v>0.74397826</v>
+      </c>
+    </row>
+    <row r="119" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B119" s="15">
+        <v>3.0000000000000058</v>
+      </c>
+      <c r="C119" s="15">
+        <f t="shared" si="9"/>
+        <v>0.66481538461538081</v>
+      </c>
+      <c r="D119" s="15">
+        <v>3.0000000000000058</v>
+      </c>
+      <c r="E119" s="15">
+        <v>0.66481555000000003</v>
+      </c>
+    </row>
+    <row r="120" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B120" s="15">
+        <v>3.1200000000000059</v>
+      </c>
+      <c r="C120" s="15">
+        <f t="shared" si="9"/>
+        <v>0.58669474953845779</v>
+      </c>
+      <c r="D120" s="15">
+        <v>3.1200000000000059</v>
+      </c>
+      <c r="E120" s="15">
+        <v>0.58669484000000005</v>
+      </c>
+    </row>
+    <row r="121" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B121" s="15">
+        <v>3.240000000000006</v>
+      </c>
+      <c r="C121" s="15">
+        <f t="shared" si="9"/>
+        <v>0.51169222399999637</v>
+      </c>
+      <c r="D121" s="15">
+        <v>3.240000000000006</v>
+      </c>
+      <c r="E121" s="15">
+        <v>0.51169240000000005</v>
+      </c>
+    </row>
+    <row r="122" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B122" s="15">
+        <v>3.3600000000000061</v>
+      </c>
+      <c r="C122" s="15">
+        <f t="shared" si="9"/>
+        <v>0.44188380061538113</v>
+      </c>
+      <c r="D122" s="15">
+        <v>3.3600000000000061</v>
+      </c>
+      <c r="E122" s="15">
+        <v>0.44188386000000002</v>
+      </c>
+    </row>
+    <row r="123" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B123" s="15">
+        <v>3.4800000000000062</v>
+      </c>
+      <c r="C123" s="15">
+        <f t="shared" si="9"/>
+        <v>0.37934547199999702</v>
+      </c>
+      <c r="D123" s="15">
+        <v>3.4800000000000062</v>
+      </c>
+      <c r="E123" s="15">
+        <v>0.37934560000000001</v>
+      </c>
+    </row>
+    <row r="124" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B124" s="15">
+        <v>3.6000000000000063</v>
+      </c>
+      <c r="C124" s="15">
+        <f t="shared" si="9"/>
+        <v>0.3261532307692282</v>
+      </c>
+      <c r="D124" s="15">
+        <v>3.6000000000000063</v>
+      </c>
+      <c r="E124" s="15">
+        <v>0.32615327999999999</v>
+      </c>
+    </row>
+    <row r="125" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B125" s="15">
+        <v>3.7200000000000064</v>
+      </c>
+      <c r="C125" s="15">
+        <f t="shared" si="9"/>
+        <v>0.28438306953845971</v>
+      </c>
+      <c r="D125" s="15">
+        <v>3.7200000000000064</v>
+      </c>
+      <c r="E125" s="15">
+        <v>0.28438314999999997</v>
+      </c>
+    </row>
+    <row r="126" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B126" s="15">
+        <v>3.8400000000000065</v>
+      </c>
+      <c r="C126" s="15">
+        <f t="shared" si="9"/>
+        <v>0.2561109809230756</v>
+      </c>
+      <c r="D126" s="15">
+        <v>3.8400000000000065</v>
+      </c>
+      <c r="E126" s="15">
+        <v>0.25611106</v>
+      </c>
+    </row>
+    <row r="127" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B127" s="15">
+        <v>3.9600000000000066</v>
+      </c>
+      <c r="C127" s="15">
+        <f t="shared" si="9"/>
+        <v>0.24341295753846093</v>
+      </c>
+      <c r="D127" s="15">
+        <v>3.9600000000000066</v>
+      </c>
+      <c r="E127" s="15">
+        <v>0.24341297000000001</v>
+      </c>
+    </row>
+    <row r="128" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B128" s="15">
+        <v>4.0800000000000063</v>
+      </c>
+      <c r="C128" s="15">
+        <f>$C$33+($M$47*(B128-$B$10))+($M$39*(B128-$B$10)^2)+($M$54*(B128-$B$10)^3)</f>
+        <v>0.24820812701538533</v>
+      </c>
+      <c r="D128" s="15">
+        <v>4.0800000000000063</v>
+      </c>
+      <c r="E128" s="15">
+        <v>0.24820812</v>
+      </c>
+    </row>
+    <row r="129" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B129" s="15">
+        <v>4.2000000000000064</v>
+      </c>
+      <c r="C129" s="15">
+        <f t="shared" ref="C129:C144" si="10">$C$33+($M$47*(B129-$B$10))+($M$39*(B129-$B$10)^2)+($M$54*(B129-$B$10)^3)</f>
+        <v>0.27059206153846316</v>
+      </c>
+      <c r="D129" s="15">
+        <v>4.2000000000000064</v>
+      </c>
+      <c r="E129" s="15">
+        <v>0.270592</v>
+      </c>
+    </row>
+    <row r="130" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B130" s="15">
+        <v>4.3200000000000065</v>
+      </c>
+      <c r="C130" s="15">
+        <f t="shared" si="10"/>
+        <v>0.30948384590769484</v>
+      </c>
+      <c r="D130" s="15">
+        <v>4.3200000000000065</v>
+      </c>
+      <c r="E130" s="15">
+        <v>0.30948371000000002</v>
+      </c>
+    </row>
+    <row r="131" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B131" s="15">
+        <v>4.4400000000000066</v>
+      </c>
+      <c r="C131" s="15">
+        <f t="shared" si="10"/>
+        <v>0.36378295680000344</v>
+      </c>
+      <c r="D131" s="15">
+        <v>4.4400000000000066</v>
+      </c>
+      <c r="E131" s="15">
+        <v>0.36378273</v>
+      </c>
+    </row>
+    <row r="132" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B132" s="15">
+        <v>4.5600000000000067</v>
+      </c>
+      <c r="C132" s="15">
+        <f t="shared" si="10"/>
+        <v>0.43238887089231198</v>
+      </c>
+      <c r="D132" s="15">
+        <v>4.5600000000000067</v>
+      </c>
+      <c r="E132" s="15">
+        <v>0.43238881000000001</v>
+      </c>
+    </row>
+    <row r="133" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B133" s="15">
+        <v>4.6800000000000068</v>
+      </c>
+      <c r="C133" s="15">
+        <f t="shared" si="10"/>
+        <v>0.51420106486154349</v>
+      </c>
+      <c r="D133" s="15">
+        <v>4.6800000000000068</v>
+      </c>
+      <c r="E133" s="15">
+        <v>0.51420093</v>
+      </c>
+    </row>
+    <row r="134" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B134" s="15">
+        <v>4.8000000000000069</v>
+      </c>
+      <c r="C134" s="15">
+        <f t="shared" si="10"/>
+        <v>0.60811901538462121</v>
+      </c>
+      <c r="D134" s="15">
+        <v>4.8000000000000069</v>
+      </c>
+      <c r="E134" s="15">
+        <v>0.60811877000000003</v>
+      </c>
+    </row>
+    <row r="135" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B135" s="15">
+        <v>4.920000000000007</v>
+      </c>
+      <c r="C135" s="15">
+        <f t="shared" si="10"/>
+        <v>0.71304219913846822</v>
+      </c>
+      <c r="D135" s="15">
+        <v>4.920000000000007</v>
+      </c>
+      <c r="E135" s="15">
+        <v>0.71304177999999996</v>
+      </c>
+    </row>
+    <row r="136" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B136" s="15">
+        <v>5.0400000000000071</v>
+      </c>
+      <c r="C136" s="15">
+        <f t="shared" si="10"/>
+        <v>0.82787009280000723</v>
+      </c>
+      <c r="D136" s="15">
+        <v>5.0400000000000071</v>
+      </c>
+      <c r="E136" s="15">
+        <v>0.82787001000000005</v>
+      </c>
+    </row>
+    <row r="137" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B137" s="15">
+        <v>5.1600000000000072</v>
+      </c>
+      <c r="C137" s="15">
+        <f t="shared" si="10"/>
+        <v>0.9515021730461618</v>
+      </c>
+      <c r="D137" s="15">
+        <v>5.1600000000000072</v>
+      </c>
+      <c r="E137" s="15">
+        <v>0.95150197000000003</v>
+      </c>
+    </row>
+    <row r="138" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B138" s="15">
+        <v>5.2800000000000074</v>
+      </c>
+      <c r="C138" s="15">
+        <f t="shared" si="10"/>
+        <v>1.0828379165538544</v>
+      </c>
+      <c r="D138" s="15">
+        <v>5.2800000000000074</v>
+      </c>
+      <c r="E138" s="15">
+        <v>1.0828376</v>
+      </c>
+    </row>
+    <row r="139" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B139" s="15">
+        <v>5.4000000000000075</v>
+      </c>
+      <c r="C139" s="15">
+        <f t="shared" si="10"/>
+        <v>1.220776800000009</v>
+      </c>
+      <c r="D139" s="15">
+        <v>5.4000000000000075</v>
+      </c>
+      <c r="E139" s="15">
+        <v>1.2207763</v>
+      </c>
+    </row>
+    <row r="140" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B140" s="15">
+        <v>5.5200000000000076</v>
+      </c>
+      <c r="C140" s="15">
+        <f t="shared" si="10"/>
+        <v>1.364218300061548</v>
+      </c>
+      <c r="D140" s="15">
+        <v>5.5200000000000076</v>
+      </c>
+      <c r="E140" s="15">
+        <v>1.3642175999999999</v>
+      </c>
+    </row>
+    <row r="141" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B141" s="15">
+        <v>5.6400000000000077</v>
+      </c>
+      <c r="C141" s="15">
+        <f t="shared" si="10"/>
+        <v>1.5120618934153944</v>
+      </c>
+      <c r="D141" s="15">
+        <v>5.6400000000000077</v>
+      </c>
+      <c r="E141" s="15">
+        <v>1.5120617000000001</v>
+      </c>
+    </row>
+    <row r="142" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B142" s="15">
+        <v>5.7600000000000078</v>
+      </c>
+      <c r="C142" s="15">
+        <f t="shared" si="10"/>
+        <v>1.6632070567384716</v>
+      </c>
+      <c r="D142" s="15">
+        <v>5.7600000000000078</v>
+      </c>
+      <c r="E142" s="15">
+        <v>1.6632066999999999</v>
+      </c>
+    </row>
+    <row r="143" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B143" s="15">
+        <v>5.8800000000000079</v>
+      </c>
+      <c r="C143" s="15">
+        <f t="shared" si="10"/>
+        <v>1.8165532667077025</v>
+      </c>
+      <c r="D143" s="15">
+        <v>5.8800000000000079</v>
+      </c>
+      <c r="E143" s="15">
+        <v>1.8165528</v>
+      </c>
+    </row>
+    <row r="144" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B144" s="15">
+        <v>6.000000000000008</v>
+      </c>
+      <c r="C144" s="15">
+        <f t="shared" si="10"/>
+        <v>1.9710000000000107</v>
+      </c>
+      <c r="D144" s="15">
+        <v>6.000000000000008</v>
+      </c>
+      <c r="E144" s="15">
+        <v>1.9709994</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="F26:M26"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>